<commit_message>
history data and live data donut
</commit_message>
<xml_diff>
--- a/DockerFiles/ExcelProduction/DownCode/DownCode.xlsx
+++ b/DockerFiles/ExcelProduction/DownCode/DownCode.xlsx
@@ -1,12 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24709"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{267F9FAC-CA05-4D4B-9D41-C1EE33F4AC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,7 +40,7 @@
     <t>Category</t>
   </si>
   <si>
-    <t>Color</t>
+    <t>color</t>
   </si>
   <si>
     <t>Holiday</t>
@@ -100,25 +115,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF6A8759"/>
       <name val="Consolas"/>
     </font>
@@ -128,7 +144,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -138,31 +154,12 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -171,61 +168,87 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -415,23 +438,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="21.0"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,15 +476,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5">
       <c r="A2" s="4">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>6</v>
@@ -465,15 +493,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5">
       <c r="A3" s="4">
-        <v>201.0</v>
+        <v>201</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="6">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>6</v>
@@ -482,15 +510,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5">
       <c r="A4" s="4">
-        <v>202.0</v>
+        <v>202</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="6">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>6</v>
@@ -499,15 +527,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5">
       <c r="A5" s="4">
-        <v>203.0</v>
+        <v>203</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
@@ -516,15 +544,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5">
       <c r="A6" s="4">
-        <v>204.0</v>
+        <v>204</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>15</v>
@@ -533,15 +561,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5">
       <c r="A7" s="4">
-        <v>205.0</v>
+        <v>205</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>15</v>
@@ -550,15 +578,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5">
       <c r="A8" s="4">
-        <v>206.0</v>
+        <v>206</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>15</v>
@@ -567,15 +595,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5">
       <c r="A9" s="4">
-        <v>207.0</v>
+        <v>207</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>15</v>
@@ -584,15 +612,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5">
       <c r="A10" s="4">
-        <v>208.0</v>
+        <v>208</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>15</v>
@@ -601,15 +629,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5">
       <c r="A11" s="4">
-        <v>209.0</v>
+        <v>209</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>15</v>
@@ -618,15 +646,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5">
       <c r="A12" s="4">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="6">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>15</v>
@@ -636,6 +664,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
</xml_diff>